<commit_message>
CIERRE 22 NOV 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/ETIQ,.LIBROS.xlsx
+++ b/01 DOCUEMENTOS/ETIQ,.LIBROS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="10335" windowHeight="4815" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="600" yWindow="105" windowWidth="10335" windowHeight="4815" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="MAS ETIQUETAS   " sheetId="9" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
   <si>
     <t>Damián Hernández Polvo</t>
   </si>
@@ -260,61 +260,13 @@
     <t>CALZADA ZAVALETA # 706</t>
   </si>
   <si>
-    <t xml:space="preserve">                       Tacos Dorados</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Semana cinco</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                        Lunes</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:               Arroz blanco</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">                               Huauzontles con queso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                           Calabacitas rellenas        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                 Tortitas de papa</t>
+    <t>IMPRESORA HPMFP137FNW     20-NOV-2023</t>
+  </si>
+  <si>
+    <t>Carne de puero salsa verde con calabazas</t>
+  </si>
+  <si>
+    <t>Norteño con espinacas, y rajas de guachinango</t>
   </si>
   <si>
     <r>
@@ -326,7 +278,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Semana dos</t>
+      <t>Semana uno</t>
     </r>
     <r>
       <rPr>
@@ -347,7 +299,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">      Lunes</t>
+      <t xml:space="preserve">      Jueves</t>
     </r>
     <r>
       <rPr>
@@ -371,7 +323,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Semana tres</t>
+      <t>Semana dos</t>
     </r>
     <r>
       <rPr>
@@ -403,7 +355,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">   Miercoles</t>
+      <t xml:space="preserve">   Sabado</t>
     </r>
     <r>
       <rPr>
@@ -414,8 +366,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>:          Arroz blanco</t>
+      <t>:          Sopa de pasta</t>
     </r>
+  </si>
+  <si>
+    <t>Pechugas al horno</t>
   </si>
   <si>
     <r>
@@ -427,7 +382,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Semana cuatro</t>
+      <t>Semana tres</t>
     </r>
     <r>
       <rPr>
@@ -459,7 +414,53 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">:        Sopa de verduras </t>
+      <t>:        Arroz blanco</t>
+    </r>
+  </si>
+  <si>
+    <t>Papas con poblano y granos de elote</t>
+  </si>
+  <si>
+    <t>Frijol con costilla de puerco</t>
+  </si>
+  <si>
+    <t>Chile guachinango con atun   (  sin capear )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Semana cinco </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Lunes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sopa de papa blanca ---Pechugas al horno c/calabaza, champiñon-cebolla morada, espinaca</t>
     </r>
   </si>
   <si>
@@ -483,7 +484,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                                                  </t>
+      <t xml:space="preserve">       </t>
     </r>
     <r>
       <rPr>
@@ -493,7 +494,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">   Lunes</t>
+      <t xml:space="preserve"> Lunes</t>
     </r>
     <r>
       <rPr>
@@ -504,14 +505,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>:            Arroz blanco</t>
+      <t>:   sopa pasta</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">                         Chiles rellenos con queso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                           Calabacitas a la mexicana</t>
+    <r>
+      <t xml:space="preserve">Semana cinco    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Viernes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:   Sopa fria Codito, con jamon y crema</t>
+    </r>
   </si>
   <si>
     <r>
@@ -519,7 +540,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -530,24 +551,21 @@
     <r>
       <rPr>
         <b/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">      Arroz verde                          </t>
+      <t xml:space="preserve">      Arroz Blanco                         </t>
     </r>
-  </si>
-  <si>
-    <t>IMPRESORA HPMFP137FNW     20-NOV-2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,14 +736,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -829,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1022,9 +1032,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1034,14 +1041,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3730,23 +3755,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="69" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="69" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="69" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" style="69" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" style="69" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="68" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="68" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="68" customWidth="1"/>
+    <col min="4" max="4" width="47" style="68" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" style="68" customWidth="1"/>
+    <col min="6" max="6" width="38.140625" style="68" customWidth="1"/>
     <col min="7" max="7" width="29.85546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" style="69" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="69"/>
+    <col min="8" max="8" width="4" style="68" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3754,22 +3782,22 @@
       <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
-        <v>88</v>
+      <c r="B2" s="77" t="s">
+        <v>90</v>
       </c>
       <c r="C2" s="34"/>
-      <c r="D2" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="70"/>
+      <c r="D2" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="70" t="s">
-        <v>77</v>
+      <c r="B3" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="C3" s="34"/>
-      <c r="D3" s="70" t="s">
-        <v>77</v>
+      <c r="D3" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="G3" s="33"/>
     </row>
@@ -3783,75 +3811,75 @@
       <c r="G4" s="33"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="68" t="s">
-        <v>82</v>
+    <row r="5" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="75" t="s">
+        <v>80</v>
       </c>
       <c r="C5" s="34"/>
-      <c r="D5" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="70"/>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="71" t="s">
+      <c r="D5" s="75" t="s">
         <v>80</v>
       </c>
+      <c r="G5" s="69"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="72" t="s">
+        <v>79</v>
+      </c>
       <c r="C6" s="34"/>
-      <c r="D6" s="71" t="s">
-        <v>80</v>
+      <c r="D6" s="72" t="s">
+        <v>79</v>
       </c>
       <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
-      <c r="D7" s="73"/>
+      <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="67" t="s">
-        <v>83</v>
+      <c r="B8" s="76" t="s">
+        <v>81</v>
       </c>
       <c r="C8" s="34"/>
-      <c r="D8" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="70"/>
+      <c r="D8" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="69"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
-        <v>81</v>
+      <c r="B9" s="73" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="34"/>
-      <c r="D9" s="39" t="s">
-        <v>81</v>
+      <c r="D9" s="73" t="s">
+        <v>82</v>
       </c>
       <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
-      <c r="D10" s="73"/>
+      <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="67" t="s">
-        <v>84</v>
+      <c r="B11" s="76" t="s">
+        <v>83</v>
       </c>
       <c r="C11" s="34"/>
-      <c r="D11" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="70"/>
+      <c r="D11" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="69"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="70"/>
+        <v>84</v>
+      </c>
+      <c r="G12" s="69"/>
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
@@ -3859,71 +3887,75 @@
       <c r="D13" s="33"/>
       <c r="G13" s="33"/>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="67" t="s">
-        <v>78</v>
+    <row r="14" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="78" t="s">
+        <v>87</v>
       </c>
       <c r="C14" s="34"/>
-      <c r="D14" s="67" t="s">
-        <v>78</v>
+      <c r="D14" s="78" t="s">
+        <v>87</v>
       </c>
       <c r="G14" s="33"/>
     </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="39" t="s">
-        <v>79</v>
-      </c>
+    <row r="15" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="74"/>
       <c r="C15" s="34"/>
-      <c r="D15" s="39" t="s">
-        <v>79</v>
-      </c>
+      <c r="D15" s="74"/>
       <c r="G15" s="33"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
-      <c r="D16" s="73"/>
+      <c r="D16" s="34"/>
       <c r="G16" s="33"/>
     </row>
-    <row r="17" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="67" t="s">
+    <row r="17" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="67" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="33"/>
-    </row>
-    <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="39" t="s">
-        <v>86</v>
-      </c>
       <c r="G18" s="33"/>
     </row>
-    <row r="19" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
       <c r="D19" s="33"/>
       <c r="G19" s="33"/>
     </row>
-    <row r="20" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="33"/>
-      <c r="D20" s="72"/>
+    <row r="20" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="79" t="s">
+        <v>88</v>
+      </c>
       <c r="G20" s="33"/>
     </row>
     <row r="21" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="68"/>
+      <c r="B21" s="69" t="s">
+        <v>86</v>
+      </c>
       <c r="C21" s="34"/>
-      <c r="D21" s="68"/>
+      <c r="D21" s="69" t="s">
+        <v>86</v>
+      </c>
       <c r="G21" s="33"/>
     </row>
     <row r="22" spans="2:7" s="34" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="B22" s="69"/>
+      <c r="D22" s="70"/>
       <c r="G22" s="33"/>
     </row>
     <row r="23" spans="2:7" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3933,7 +3965,7 @@
     <row r="24" spans="2:7" s="34" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B24" s="67"/>
       <c r="D24" s="67"/>
-      <c r="G24" s="70"/>
+      <c r="G24" s="69"/>
     </row>
     <row r="25" spans="2:7" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="39"/>
@@ -3953,9 +3985,9 @@
       <c r="D28" s="39"/>
     </row>
     <row r="29" spans="2:7" s="34" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="G29" s="70"/>
+      <c r="B29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="G29" s="69"/>
     </row>
     <row r="30" spans="2:7" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B30" s="44"/>
@@ -3974,9 +4006,9 @@
     </row>
     <row r="33" spans="2:7" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:7" s="34" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="G34" s="70"/>
+      <c r="B34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="G34" s="69"/>
     </row>
     <row r="35" spans="2:7" s="34" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B35" s="44"/>
@@ -4016,7 +4048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4029,8 +4061,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="74" t="s">
-        <v>89</v>
+      <c r="D2" s="71" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>